<commit_message>
Aggiunta tabella dei requisiti
</commit_message>
<xml_diff>
--- a/Tabella dei Requisiti.xlsx
+++ b/Tabella dei Requisiti.xlsx
@@ -1147,9 +1147,7 @@
       <c r="X23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="3">
-        <v>22.0</v>
-      </c>
+      <c r="A24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1175,10 +1173,10 @@
     </row>
     <row r="25">
       <c r="A25" s="3">
-        <v>23.0</v>
+        <v>22.0</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1202,7 +1200,7 @@
     </row>
     <row r="26">
       <c r="A26" s="3">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1229,7 +1227,7 @@
     </row>
     <row r="27">
       <c r="A27" s="3">
-        <v>25.0</v>
+        <v>24.0</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1256,9 +1254,8 @@
     </row>
     <row r="28">
       <c r="A28" s="3">
-        <v>26.0</v>
+        <v>25.0</v>
       </c>
-      <c r="B28" s="3"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1284,7 +1281,7 @@
     </row>
     <row r="29">
       <c r="A29" s="3">
-        <v>27.0</v>
+        <v>26.0</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
@@ -1312,7 +1309,7 @@
     </row>
     <row r="30">
       <c r="A30" s="3">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
@@ -1340,7 +1337,7 @@
     </row>
     <row r="31">
       <c r="A31" s="3">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
@@ -1368,8 +1365,9 @@
     </row>
     <row r="32">
       <c r="A32" s="3">
-        <v>30.0</v>
+        <v>29.0</v>
       </c>
+      <c r="B32" s="3"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1394,8 +1392,9 @@
       <c r="X32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="3">
+        <v>30.0</v>
+      </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1914,7 +1913,7 @@
       <c r="X52" s="4"/>
     </row>
     <row r="53">
-      <c r="A53" s="4"/>
+      <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -26587,6 +26586,32 @@
       <c r="W1001" s="4"/>
       <c r="X1001" s="4"/>
     </row>
+    <row r="1002">
+      <c r="A1002" s="4"/>
+      <c r="B1002" s="4"/>
+      <c r="C1002" s="4"/>
+      <c r="D1002" s="4"/>
+      <c r="E1002" s="4"/>
+      <c r="F1002" s="4"/>
+      <c r="G1002" s="4"/>
+      <c r="H1002" s="4"/>
+      <c r="I1002" s="4"/>
+      <c r="J1002" s="4"/>
+      <c r="K1002" s="4"/>
+      <c r="L1002" s="4"/>
+      <c r="M1002" s="4"/>
+      <c r="N1002" s="4"/>
+      <c r="O1002" s="4"/>
+      <c r="P1002" s="4"/>
+      <c r="Q1002" s="4"/>
+      <c r="R1002" s="4"/>
+      <c r="S1002" s="4"/>
+      <c r="T1002" s="4"/>
+      <c r="U1002" s="4"/>
+      <c r="V1002" s="4"/>
+      <c r="W1002" s="4"/>
+      <c r="X1002" s="4"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>